<commit_message>
Actualizacion del esquema general de la aplicacion seguimiento de facturas
</commit_message>
<xml_diff>
--- a/DiccionarioDeDatosSeguimientoDeFacturas.xlsx
+++ b/DiccionarioDeDatosSeguimientoDeFacturas.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\segfact\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="11550"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
   <si>
     <t>Diccionario de datos para Aplicación de Seguimiento a facturas</t>
   </si>
@@ -33,9 +38,6 @@
     <t>NumDiag</t>
   </si>
   <si>
-    <t>Placa</t>
-  </si>
-  <si>
     <t>NumFactura</t>
   </si>
   <si>
@@ -126,9 +128,6 @@
     <t>CelVentas</t>
   </si>
   <si>
-    <t>Direccion</t>
-  </si>
-  <si>
     <t>DireccionAtencion</t>
   </si>
   <si>
@@ -147,9 +146,6 @@
     <t>Fecha</t>
   </si>
   <si>
-    <t>Vehiculos</t>
-  </si>
-  <si>
     <t>Cadena</t>
   </si>
   <si>
@@ -159,9 +155,6 @@
     <t>IdEstatus</t>
   </si>
   <si>
-    <t>IdVehiculo</t>
-  </si>
-  <si>
     <t>Correo</t>
   </si>
   <si>
@@ -183,39 +176,6 @@
     <t>RFC</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>Modelo</t>
-  </si>
-  <si>
-    <t>Motor</t>
-  </si>
-  <si>
-    <t>Puertas</t>
-  </si>
-  <si>
-    <t>Cilindros</t>
-  </si>
-  <si>
-    <t>Transmision</t>
-  </si>
-  <si>
-    <t>IdTipo</t>
-  </si>
-  <si>
-    <t>Tipos</t>
-  </si>
-  <si>
-    <t>Año</t>
-  </si>
-  <si>
-    <t>Serie</t>
-  </si>
-  <si>
     <t>csc</t>
   </si>
   <si>
@@ -234,19 +194,7 @@
     <t>fk_Vale_DepEnt</t>
   </si>
   <si>
-    <t>fk_Vale_Vehiculos</t>
-  </si>
-  <si>
     <t>fk_Vale_Proveedor</t>
-  </si>
-  <si>
-    <t>fk_Vehiculos_Tipo</t>
-  </si>
-  <si>
-    <t>fk_Vehiculos_EntDep</t>
-  </si>
-  <si>
-    <t>IdEntDep</t>
   </si>
 </sst>
 </file>
@@ -320,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -333,6 +281,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,6 +294,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -390,7 +345,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -425,7 +380,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -637,7 +592,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,29 +622,29 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -700,16 +655,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -717,22 +672,22 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I5">
-        <v>8</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -740,22 +695,22 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -766,7 +721,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -775,13 +730,13 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I7">
-        <v>20</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -792,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -801,13 +756,13 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -815,19 +770,19 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F9">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I9">
         <v>20</v>
@@ -838,22 +793,25 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
       </c>
       <c r="F10">
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I10">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -864,22 +822,19 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F11">
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I11">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -890,19 +845,19 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F12">
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -910,22 +865,22 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F13">
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -933,22 +888,22 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F14">
         <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I14">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -961,661 +916,440 @@
       <c r="C15" t="s">
         <v>41</v>
       </c>
+      <c r="D15">
+        <v>255</v>
+      </c>
       <c r="F15">
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I15">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16">
-        <v>255</v>
-      </c>
       <c r="F16">
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
         <v>41</v>
       </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
       <c r="F17">
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="H17" t="s">
         <v>41</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>71</v>
+        <v>57</v>
+      </c>
+      <c r="F18">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>72</v>
+      <c r="F19">
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>73</v>
+      <c r="A20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20">
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21">
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>40</v>
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22">
+        <v>255</v>
       </c>
       <c r="E22" s="6"/>
-      <c r="F22" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" t="s">
-        <v>41</v>
-      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D24">
         <v>255</v>
       </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H24" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24">
-        <v>20</v>
-      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D25">
-        <v>20</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D26">
-        <v>255</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27">
         <v>5</v>
-      </c>
-      <c r="B27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27">
-        <v>255</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D28">
-        <v>10</v>
-      </c>
-      <c r="F28">
-        <v>2</v>
-      </c>
-      <c r="G28" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" t="s">
-        <v>44</v>
-      </c>
-      <c r="I28">
-        <v>255</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D29">
-        <v>5</v>
-      </c>
-      <c r="F29">
-        <v>3</v>
-      </c>
-      <c r="G29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29">
-        <v>255</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D30">
-        <v>5</v>
-      </c>
-      <c r="F30">
-        <v>4</v>
-      </c>
-      <c r="G30" t="s">
-        <v>38</v>
-      </c>
-      <c r="H30" t="s">
-        <v>44</v>
-      </c>
-      <c r="I30">
-        <v>255</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D31">
         <v>20</v>
       </c>
-      <c r="F31">
-        <v>5</v>
-      </c>
-      <c r="G31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I31">
-        <v>255</v>
-      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32">
         <v>10</v>
       </c>
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32">
-        <v>100</v>
-      </c>
-      <c r="F32">
-        <v>6</v>
-      </c>
-      <c r="G32" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" t="s">
-        <v>44</v>
-      </c>
-      <c r="I32">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
         <v>20</v>
       </c>
-      <c r="F33">
-        <v>7</v>
-      </c>
-      <c r="G33" t="s">
-        <v>67</v>
-      </c>
-      <c r="H33" t="s">
-        <v>44</v>
-      </c>
-      <c r="I33">
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>12</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
         <v>26</v>
       </c>
-      <c r="C34" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34">
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37">
         <v>10</v>
       </c>
-      <c r="F34">
-        <v>8</v>
-      </c>
-      <c r="G34" t="s">
-        <v>68</v>
-      </c>
-      <c r="H34" t="s">
-        <v>44</v>
-      </c>
-      <c r="I34">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>13</v>
-      </c>
-      <c r="B35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35">
-        <v>15</v>
-      </c>
-      <c r="F35">
-        <v>9</v>
-      </c>
-      <c r="G35" t="s">
-        <v>69</v>
-      </c>
-      <c r="H35" t="s">
-        <v>44</v>
-      </c>
-      <c r="I35">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>14</v>
-      </c>
-      <c r="B36" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36">
-        <v>255</v>
-      </c>
-      <c r="F36">
-        <v>10</v>
-      </c>
-      <c r="G36" t="s">
-        <v>31</v>
-      </c>
-      <c r="H36" t="s">
-        <v>44</v>
-      </c>
-      <c r="I36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>15</v>
-      </c>
-      <c r="B37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37">
-        <v>100</v>
-      </c>
-      <c r="F37">
-        <v>11</v>
-      </c>
-      <c r="G37" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" t="s">
-        <v>44</v>
-      </c>
-      <c r="I37">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>20</v>
       </c>
-      <c r="F38">
-        <v>12</v>
-      </c>
-      <c r="G38" t="s">
-        <v>26</v>
-      </c>
-      <c r="H38" t="s">
-        <v>44</v>
-      </c>
-      <c r="I38">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>17</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>27</v>
       </c>
-      <c r="C39" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39">
-        <v>10</v>
-      </c>
-      <c r="F39">
-        <v>13</v>
-      </c>
-      <c r="G39" t="s">
-        <v>20</v>
-      </c>
-      <c r="H39" t="s">
-        <v>44</v>
-      </c>
-      <c r="I39">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>18</v>
-      </c>
-      <c r="B40" t="s">
-        <v>24</v>
-      </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D40">
-        <v>15</v>
-      </c>
-      <c r="F40">
-        <v>14</v>
-      </c>
-      <c r="G40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H40" t="s">
-        <v>44</v>
-      </c>
-      <c r="I40">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>19</v>
-      </c>
-      <c r="B41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41">
         <v>255</v>
       </c>
-      <c r="F41">
-        <v>15</v>
-      </c>
-      <c r="G41" t="s">
-        <v>33</v>
-      </c>
-      <c r="H41" t="s">
-        <v>44</v>
-      </c>
-      <c r="I41">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>20</v>
-      </c>
-      <c r="B42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42">
-        <v>255</v>
-      </c>
-      <c r="F42">
-        <v>16</v>
-      </c>
-      <c r="G42" t="s">
-        <v>34</v>
-      </c>
-      <c r="H42" t="s">
-        <v>44</v>
-      </c>
-      <c r="I42">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F43">
-        <v>17</v>
-      </c>
-      <c r="G43" t="s">
-        <v>35</v>
-      </c>
-      <c r="H43" t="s">
-        <v>44</v>
-      </c>
-      <c r="I43">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E44" s="6"/>
-      <c r="F44">
-        <v>18</v>
-      </c>
-      <c r="G44" t="s">
-        <v>48</v>
-      </c>
-      <c r="H44" t="s">
-        <v>44</v>
-      </c>
-      <c r="I44">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D46">
         <v>20</v>

</xml_diff>